<commit_message>
Move from version 3.5.0 of the espressif32 platform to version 6.5.0 so we're getting the latest and greatest Move the call to Wire.begin(); _very_ early or it doesn't work with the latest (6.5.0) platform Have a debug and a separate JTAG build as I still can't get JTAG debugging to work
</commit_message>
<xml_diff>
--- a/Related chip information/ESP32 pin assignments.xlsx
+++ b/Related chip information/ESP32 pin assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ada\Related chip information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41BD608-E5FE-42CC-B7CA-BB918CAF8605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313EE8BE-1B23-4707-A177-B2C398E21E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21960" yWindow="765" windowWidth="26010" windowHeight="20985" xr2:uid="{56C63F47-42D5-4463-8DA8-24EC799EC9D3}"/>
+    <workbookView xWindow="1170" yWindow="615" windowWidth="26010" windowHeight="20985" xr2:uid="{56C63F47-42D5-4463-8DA8-24EC799EC9D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="113">
   <si>
     <t>Vin 5V</t>
   </si>
@@ -273,13 +273,126 @@
   </si>
   <si>
     <t>JTAG 6 (TDO)</t>
+  </si>
+  <si>
+    <t>Wiring Connections</t>
+  </si>
+  <si>
+    <t>ESP-Prog JTAG 10-Pin Connector</t>
+  </si>
+  <si>
+    <t>JTAG Signal</t>
+  </si>
+  <si>
+    <t>ESP32 Pin</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>VDD</t>
+  </si>
+  <si>
+    <t>Positive Supply Voltage — Power supply for JTAG interface drivers</t>
+  </si>
+  <si>
+    <t>Digital ground</t>
+  </si>
+  <si>
+    <t>TMS</t>
+  </si>
+  <si>
+    <t>GPIO14</t>
+  </si>
+  <si>
+    <t>Test Mode State</t>
+  </si>
+  <si>
+    <t>TCK</t>
+  </si>
+  <si>
+    <t>GPIO13</t>
+  </si>
+  <si>
+    <t>JTAG Return Test Clock</t>
+  </si>
+  <si>
+    <t>TDO</t>
+  </si>
+  <si>
+    <t>GPIO15</t>
+  </si>
+  <si>
+    <t>Test Data Out</t>
+  </si>
+  <si>
+    <t>TDI</t>
+  </si>
+  <si>
+    <t>GPIO12</t>
+  </si>
+  <si>
+    <t>Test Data In</t>
+  </si>
+  <si>
+    <r>
+      <t>Wiring Connections</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF2980B9"/>
+        <rFont val="FontAwesome"/>
+      </rPr>
+      <t></t>
+    </r>
+  </si>
+  <si>
+    <t>ESP32-S2 and ESP32-S3 Pin</t>
+  </si>
+  <si>
+    <t>ESP32-C2, ESP32-C3, ESP32-C6, and ESP32-P4 Pin</t>
+  </si>
+  <si>
+    <t>ESP32-H2 Pin</t>
+  </si>
+  <si>
+    <t>GPIO42</t>
+  </si>
+  <si>
+    <t>GPIO4</t>
+  </si>
+  <si>
+    <t>GPIO2</t>
+  </si>
+  <si>
+    <t>GPIO39</t>
+  </si>
+  <si>
+    <t>GPIO6</t>
+  </si>
+  <si>
+    <t>GPIO40</t>
+  </si>
+  <si>
+    <t>GPIO7</t>
+  </si>
+  <si>
+    <t>GPIO3</t>
+  </si>
+  <si>
+    <t>GPIO41</t>
+  </si>
+  <si>
+    <t>GPIO5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,19 +401,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF404040"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF6A9955"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <color rgb="FF2980B9"/>
+      <name val="FontAwesome"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF404040"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lato"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFC586C0"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <color theme="1"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,8 +466,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F6F6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -334,11 +499,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE1E4E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE1E4E5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE1E4E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE1E4E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE1E4E5"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFE1E4E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE1E4E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE1E4E5"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFE1E4E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -352,14 +557,46 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -379,16 +616,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1495426</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>27215</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>523876</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>151040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -411,12 +648,134 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609601" y="4572001"/>
+          <a:off x="8181976" y="4362451"/>
           <a:ext cx="4343400" cy="5170714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2028825</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>1666875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBDC9ADD-6E11-90A9-8D71-1D5A0739DC02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7924800" y="10229850"/>
+          <a:ext cx="3257550" cy="3133725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>29584</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BB81108-D7AA-40AF-BD5C-A93C0438E154}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1248784" y="4791075"/>
+          <a:ext cx="2446915" cy="2305050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -741,13 +1100,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3D7790-DAF5-429B-A1FC-5D7BE5EFA8F6}">
-  <dimension ref="B2:L32"/>
+  <dimension ref="B2:L62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.5703125" bestFit="1" customWidth="1"/>
@@ -755,7 +1114,7 @@
     <col min="12" max="12" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -787,7 +1146,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -803,7 +1162,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -819,7 +1178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -843,7 +1202,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -869,7 +1228,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -895,7 +1254,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -919,7 +1278,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -933,7 +1292,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -959,7 +1318,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -985,7 +1344,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -1014,7 +1373,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -1037,7 +1396,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -1066,7 +1425,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -1076,7 +1435,7 @@
       <c r="D15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="5" t="s">
         <v>76</v>
       </c>
       <c r="F15" t="s">
@@ -1095,7 +1454,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -1114,7 +1473,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -1124,7 +1483,7 @@
       <c r="D17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="6" t="s">
         <v>77</v>
       </c>
       <c r="H17" t="s">
@@ -1143,7 +1502,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -1165,14 +1524,14 @@
       <c r="J18" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="7" t="s">
         <v>78</v>
       </c>
       <c r="L18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -1198,7 +1557,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -1224,7 +1583,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -1246,23 +1605,289 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C31" s="6"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C32" s="6"/>
+    <row r="24" spans="2:12">
+      <c r="C24" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="181.5" customHeight="1">
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="2:12" ht="16.5" thickBot="1">
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="2:12" ht="86.25" thickBot="1">
+      <c r="C27" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="15.75" thickBot="1">
+      <c r="C28" s="10">
+        <v>1</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="15.75" thickBot="1">
+      <c r="C29" s="11">
+        <v>3</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="15.75" thickBot="1">
+      <c r="C30" s="10">
+        <v>2</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="15.75" thickBot="1">
+      <c r="C31" s="11">
+        <v>4</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="15.75" thickBot="1">
+      <c r="C32" s="10">
+        <v>6</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" ht="15.75" thickBot="1">
+      <c r="C33" s="11">
+        <v>8</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="23.25">
+      <c r="B54" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="16.5" thickBot="1">
+      <c r="B55" s="8"/>
+    </row>
+    <row r="56" spans="2:8" ht="86.25" thickBot="1">
+      <c r="B56" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="171.75" thickBot="1">
+      <c r="B57" s="10">
+        <v>1</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H57" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="29.25" thickBot="1">
+      <c r="B58" s="11">
+        <v>3</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H58" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="43.5" thickBot="1">
+      <c r="B59" s="10">
+        <v>2</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H59" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="57.75" thickBot="1">
+      <c r="B60" s="11">
+        <v>4</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H60" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="43.5" thickBot="1">
+      <c r="B61" s="10">
+        <v>6</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="29.25" thickBot="1">
+      <c r="B62" s="11">
+        <v>8</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F62" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H62" s="13" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C24" r:id="rId1" location="debugging-tool-esp-prog" xr:uid="{167A5285-DC89-488D-9FCD-3AA8657AEDB3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>